<commit_message>
Commnents updated and excel file updated
</commit_message>
<xml_diff>
--- a/CollectionsIMP.xlsx
+++ b/CollectionsIMP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tutorials\Java-Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFB6A828-8984-48BC-AFA9-2842DE6DFF2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9C002A-D41C-4C59-B014-869AE3D42988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{EE89781A-D524-4CC3-A6A1-C0C14AEF8FF2}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{EE89781A-D524-4CC3-A6A1-C0C14AEF8FF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
   <si>
     <t xml:space="preserve">Set </t>
   </si>
@@ -94,19 +94,46 @@
   </si>
   <si>
     <t>LinkedList</t>
+  </si>
+  <si>
+    <t>ArrayList</t>
+  </si>
+  <si>
+    <t>LinkedHashMap</t>
+  </si>
+  <si>
+    <t>TreehMap</t>
+  </si>
+  <si>
+    <t>If we are having duplicate keys then the latest value(value which is added last)of the key will be printed</t>
+  </si>
+  <si>
+    <t>We cannot add null at the key if we added null value to key, we will get nullPointerException</t>
+  </si>
+  <si>
+    <t>Map</t>
+  </si>
+  <si>
+    <t>Collection</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color theme="1"/>
+      <name val="Fira Code"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="10">
@@ -192,9 +219,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -203,6 +229,11 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB2A3A7B-2C0C-4481-BDE5-772EA563F8FF}">
-  <dimension ref="A2:D11"/>
+  <dimension ref="A2:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,142 +565,203 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>